<commit_message>
Fix #6770 - Modify nutrient and packagingMaterial exports
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/ExportNutrients.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/ExportNutrients.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Nutriments" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Nutriments!$B$3:$AL$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Nutriments!$B$3:$AV$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Nutriments!$B$3:$AL$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Nutriments!$B$3:$AV$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Nutriments!$B$3:$AV$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Nutriments!$B$3:$AV$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Nutriments!$B$3:$AV$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Nutriments!$B$3:$AV$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -66,7 +66,7 @@
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "ENER-E14"]_bcpg:nutListValue</t>
   </si>
   <si>
-    <t xml:space="preserve">excel|IF(ISBLANK(J2),IF(ISBLANK(I2),"",I2),J2)</t>
+    <t xml:space="preserve">excel|IF(J2="",IF(I2="","",I2),J2)</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "ENER-KJO"]_bcpg:nutListFormulatedValue</t>
@@ -75,7 +75,7 @@
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "ENER-KJO"]_bcpg:nutListValue</t>
   </si>
   <si>
-    <t xml:space="preserve">excel|IF(ISBLANK(M2),IF(ISBLANK(L2),"",L2),M2)</t>
+    <t xml:space="preserve">excel|IF(M2="",IF(L2="","",L2),M2)</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "FAT"]_bcpg:nutListFormulatedValue</t>
@@ -84,7 +84,7 @@
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "FAT"]_bcpg:nutListValue</t>
   </si>
   <si>
-    <t xml:space="preserve">excel|IF(ISBLANK(P2),IF(ISBLANK(O2),"",O2),P2)</t>
+    <t xml:space="preserve">excel|IF(P2="",IF(O2="","",O2),P2)</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "FASAT"]_bcpg:nutListFormulatedValue</t>
@@ -93,7 +93,7 @@
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "FASAT"]_bcpg:nutListValue</t>
   </si>
   <si>
-    <t xml:space="preserve">excel|IF(ISBLANK(S2),IF(ISBLANK(R2),"",R2),S2)</t>
+    <t xml:space="preserve">excel|IF(S2="",IF(R2="","",R2),S2)</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "CHOAVL"]_bcpg:nutListFormulatedValue</t>
@@ -102,7 +102,7 @@
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "CHOAVL"]_bcpg:nutListValue</t>
   </si>
   <si>
-    <t xml:space="preserve">excel|IF(ISBLANK(V2),IF(ISBLANK(U2),"",U2),V2)</t>
+    <t xml:space="preserve">excel|IF(V2="",IF(U2="","",U2),V2)</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "SUGAR"]_bcpg:nutListFormulatedValue</t>
@@ -111,7 +111,7 @@
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "SUGAR"]_bcpg:nutListValue</t>
   </si>
   <si>
-    <t xml:space="preserve">excel|IF(ISBLANK(Y2),IF(ISBLANK(X2),"",X2),Y2)</t>
+    <t xml:space="preserve">excel|IF(Y2="",IF(X2="","",X2),Y2)</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "PRO-"]_bcpg:nutListFormulatedValue</t>
@@ -120,7 +120,7 @@
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "PRO-"]_bcpg:nutListValue</t>
   </si>
   <si>
-    <t xml:space="preserve">excel|IF(ISBLANK(AB2),IF(ISBLANK(AA2),"",AA2),AB2)</t>
+    <t xml:space="preserve">excel|IF(AB2="",IF(AA2="","",AA2),AB2)</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "FIBTG"]_bcpg:nutListFormulatedValue</t>
@@ -129,7 +129,7 @@
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "FIBTG"]_bcpg:nutListValue</t>
   </si>
   <si>
-    <t xml:space="preserve">excel|IF(ISBLANK(AE2),IF(ISBLANK(AD2),"",AD2),AE2)</t>
+    <t xml:space="preserve">excel|IF(AE2="",IF(AD2="","",AD2),AE2)</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "NA"]_bcpg:nutListFormulatedValue</t>
@@ -138,7 +138,7 @@
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "NA"]_bcpg:nutListValue</t>
   </si>
   <si>
-    <t xml:space="preserve">excel|IF(ISBLANK(AH2),IF(ISBLANK(AG2),"",AG2),AH2)</t>
+    <t xml:space="preserve">excel|IF(AH2="",IF(AG2="","",AG2),AH2)</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "NACL"]_bcpg:nutListFormulatedValue</t>
@@ -147,7 +147,7 @@
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "NACL"]_bcpg:nutListValue</t>
   </si>
   <si>
-    <t xml:space="preserve">excel|IF(ISBLANK(AK2),IF(ISBLANK(AJ2),"",AJ2),AK2)</t>
+    <t xml:space="preserve">excel|IF(AK2="",IF(AJ2="","",AJ2),AK2)</t>
   </si>
   <si>
     <t xml:space="preserve">#</t>
@@ -463,10 +463,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -476,34 +472,33 @@
   <dimension ref="A1:BI3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="8" min="2" style="0" width="10.25"/>
+    <col collapsed="false" hidden="false" max="8" min="2" style="0" width="9.98979591836735"/>
     <col collapsed="false" hidden="true" max="10" min="9" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.46938775510204"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="true" max="13" min="12" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.46938775510204"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="true" max="16" min="15" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.46938775510204"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="true" max="19" min="18" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.46938775510204"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="true" max="22" min="21" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="6.46938775510204"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="true" max="25" min="24" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="6.46938775510204"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="true" max="28" min="27" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.46938775510204"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="true" max="31" min="30" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="6.46938775510204"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="true" max="34" min="33" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="6.46938775510204"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="true" max="37" min="36" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="93" min="38" style="0" width="6.46938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="94" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="93" min="38" style="0" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -554,7 +549,7 @@
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="23.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="103.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
@@ -820,7 +815,6 @@
       <c r="AV3" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:AL3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -828,6 +822,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>